<commit_message>
I got my version of the single function
</commit_message>
<xml_diff>
--- a/CH-055 Warehouse Management_1.xlsx
+++ b/CH-055 Warehouse Management_1.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="14_{A6DC8524-85D4-4049-AFC2-E49ABD8B82CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DBADB78-6C61-4DBB-9F8F-261D7812841F}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="14_{A6DC8524-85D4-4049-AFC2-E49ABD8B82CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F59CD413-7BF5-4D04-AA9F-72F0AD0CEC5E}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="MyFirstWack" sheetId="2" r:id="rId2"/>
     <sheet name="Alternate" sheetId="4" r:id="rId3"/>
+    <sheet name="MySingleFunction" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Alternate!$B$2:$E$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">MyFirstWack!$H$3:$I$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">MySingleFunction!$B$2:$E$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$E$19</definedName>
     <definedName name="_O">MyFirstWack!$C$3:$C$19</definedName>
     <definedName name="_P">MyFirstWack!$D$3:$D$19</definedName>
@@ -70,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="28">
   <si>
     <t>Result</t>
   </si>
@@ -160,6 +162,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0;;"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -563,7 +568,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -655,19 +660,9 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
@@ -683,6 +678,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Intro_Hd" xfId="2" xr:uid="{9EC2CC4D-A0B5-4F72-80C1-FD5AC0757E0D}"/>
@@ -1394,18 +1419,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="H1" s="35" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="H1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -1790,8 +1815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B3129E-AB4A-4761-A90B-3C130039CE03}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="C5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11:Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -1811,18 +1836,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="H1" s="35" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="H1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -2017,19 +2042,19 @@
       <c r="E11" s="20">
         <v>-3</v>
       </c>
-      <c r="H11" s="43" t="s">
+      <c r="H11" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="44" t="s">
+      <c r="I11" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="44" t="s">
+      <c r="J11" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="44" t="s">
+      <c r="K11" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="L11" s="45" t="s">
+      <c r="L11" s="41" t="s">
         <v>13</v>
       </c>
       <c r="N11" s="15"/>
@@ -2058,23 +2083,23 @@
       <c r="E12" s="20">
         <v>2</v>
       </c>
-      <c r="H12" s="38" cm="1">
+      <c r="H12" s="34" cm="1">
         <f t="array" ref="H12:H19">_xlfn.UNIQUE(C3:C19)</f>
         <v>1</v>
       </c>
-      <c r="I12" s="39">
+      <c r="I12" s="35">
         <f>SUMIF(C3:C19,"="&amp;H12,E3:E19)</f>
         <v>0</v>
       </c>
-      <c r="J12" s="46" t="str" cm="1">
+      <c r="J12" s="42" t="str" cm="1">
         <f t="array" ref="J12:J19">_xlfn.MAP(_xlfn.ANCHORARRAY(H12),_xlfn.LAMBDA(_xlpm.A,_xlfn.TAKE((_xlfn._xlws.FILTER(_P&amp;YEAR(_Y),_O=_xlpm.A)),1)))</f>
         <v>B2022</v>
       </c>
-      <c r="K12" s="39" t="str" cm="1">
+      <c r="K12" s="35" t="str" cm="1">
         <f t="array" ref="K12:K17">_xlfn.UNIQUE(_xlfn.ANCHORARRAY(J12))</f>
         <v>B2022</v>
       </c>
-      <c r="L12" s="40" cm="1">
+      <c r="L12" s="36" cm="1">
         <f t="array" ref="L12:L17">_xlfn.MAP(_xlfn.ANCHORARRAY(K12),_xlfn.LAMBDA(_xlpm.A,SUM(_xlfn._xlws.FILTER(I12:I19,_xlfn.ANCHORARRAY(J12)=_xlpm.A))))</f>
         <v>0</v>
       </c>
@@ -2082,15 +2107,15 @@
         <f t="array" ref="N12:N14">_xlfn._xlws.SORT(_xlfn.UNIQUE(LEFT(_xlfn.ANCHORARRAY(K12),1)))</f>
         <v>A</v>
       </c>
-      <c r="O12" s="4" cm="1">
+      <c r="O12" s="46" cm="1">
         <f t="array" ref="O12">_xlfn.XLOOKUP($N12&amp;O$11,_xlfn.ANCHORARRAY($K$12),_xlfn.ANCHORARRAY($L$12),"")</f>
         <v>0</v>
       </c>
-      <c r="P12" s="4" cm="1">
+      <c r="P12" s="46" cm="1">
         <f t="array" ref="P12">_xlfn.XLOOKUP($N12&amp;P$11,_xlfn.ANCHORARRAY($K$12),_xlfn.ANCHORARRAY($L$12),"")</f>
         <v>4</v>
       </c>
-      <c r="Q12" s="18" t="str" cm="1">
+      <c r="Q12" s="47" t="str" cm="1">
         <f t="array" ref="Q12">_xlfn.XLOOKUP($N12&amp;Q$11,_xlfn.ANCHORARRAY($K$12),_xlfn.ANCHORARRAY($L$12),"")</f>
         <v/>
       </c>
@@ -2109,34 +2134,34 @@
       <c r="E13" s="27">
         <v>-1</v>
       </c>
-      <c r="H13" s="38">
+      <c r="H13" s="34">
         <v>2</v>
       </c>
-      <c r="I13" s="39">
+      <c r="I13" s="35">
         <f t="shared" ref="I13:I19" si="0">SUMIF(C4:C20,"="&amp;H13,E4:E20)</f>
         <v>7</v>
       </c>
-      <c r="J13" s="39" t="str">
+      <c r="J13" s="35" t="str">
         <v>C2022</v>
       </c>
-      <c r="K13" s="39" t="str">
+      <c r="K13" s="35" t="str">
         <v>C2022</v>
       </c>
-      <c r="L13" s="40">
+      <c r="L13" s="36">
         <v>7</v>
       </c>
       <c r="N13" s="5" t="str">
         <v>B</v>
       </c>
-      <c r="O13" s="28" cm="1">
+      <c r="O13" s="48" cm="1">
         <f t="array" ref="O13">_xlfn.XLOOKUP($N13&amp;O$11,_xlfn.ANCHORARRAY($K$12),_xlfn.ANCHORARRAY($L$12),"")</f>
         <v>0</v>
       </c>
-      <c r="P13" s="5" t="str" cm="1">
+      <c r="P13" s="49" t="str" cm="1">
         <f t="array" ref="P13">_xlfn.XLOOKUP($N13&amp;P$11,_xlfn.ANCHORARRAY($K$12),_xlfn.ANCHORARRAY($L$12),"")</f>
         <v/>
       </c>
-      <c r="Q13" s="29" cm="1">
+      <c r="Q13" s="50" cm="1">
         <f t="array" ref="Q13">_xlfn.XLOOKUP($N13&amp;Q$11,_xlfn.ANCHORARRAY($K$12),_xlfn.ANCHORARRAY($L$12),"")</f>
         <v>1</v>
       </c>
@@ -2155,34 +2180,34 @@
       <c r="E14" s="20">
         <v>-1</v>
       </c>
-      <c r="H14" s="38">
+      <c r="H14" s="34">
         <v>3</v>
       </c>
-      <c r="I14" s="39">
+      <c r="I14" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J14" s="39" t="str">
+      <c r="J14" s="35" t="str">
         <v>A2022</v>
       </c>
-      <c r="K14" s="39" t="str">
+      <c r="K14" s="35" t="str">
         <v>A2022</v>
       </c>
-      <c r="L14" s="40">
+      <c r="L14" s="36">
         <v>0</v>
       </c>
       <c r="N14" s="7" t="str">
         <v>C</v>
       </c>
-      <c r="O14" s="7" cm="1">
+      <c r="O14" s="51" cm="1">
         <f t="array" ref="O14">_xlfn.XLOOKUP($N14&amp;O$11,_xlfn.ANCHORARRAY($K$12),_xlfn.ANCHORARRAY($L$12),"")</f>
         <v>7</v>
       </c>
-      <c r="P14" s="7" cm="1">
+      <c r="P14" s="51" cm="1">
         <f t="array" ref="P14">_xlfn.XLOOKUP($N14&amp;P$11,_xlfn.ANCHORARRAY($K$12),_xlfn.ANCHORARRAY($L$12),"")</f>
         <v>2</v>
       </c>
-      <c r="Q14" s="19" t="str" cm="1">
+      <c r="Q14" s="52" t="str" cm="1">
         <f t="array" ref="Q14">_xlfn.XLOOKUP($N14&amp;Q$11,_xlfn.ANCHORARRAY($K$12),_xlfn.ANCHORARRAY($L$12),"")</f>
         <v/>
       </c>
@@ -2201,20 +2226,20 @@
       <c r="E15" s="20">
         <v>-2</v>
       </c>
-      <c r="H15" s="38">
+      <c r="H15" s="34">
         <v>4</v>
       </c>
-      <c r="I15" s="39">
+      <c r="I15" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J15" s="39" t="str">
+      <c r="J15" s="35" t="str">
         <v>A2022</v>
       </c>
-      <c r="K15" s="39" t="str">
+      <c r="K15" s="35" t="str">
         <v>A2023</v>
       </c>
-      <c r="L15" s="40">
+      <c r="L15" s="36">
         <v>4</v>
       </c>
     </row>
@@ -2232,20 +2257,20 @@
       <c r="E16" s="27">
         <v>-2</v>
       </c>
-      <c r="H16" s="38">
-        <v>5</v>
-      </c>
-      <c r="I16" s="39">
+      <c r="H16" s="34">
+        <v>5</v>
+      </c>
+      <c r="I16" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J16" s="39" t="str">
+      <c r="J16" s="35" t="str">
         <v>C2022</v>
       </c>
-      <c r="K16" s="39" t="str">
+      <c r="K16" s="35" t="str">
         <v>C2023</v>
       </c>
-      <c r="L16" s="40">
+      <c r="L16" s="36">
         <v>2</v>
       </c>
     </row>
@@ -2263,20 +2288,20 @@
       <c r="E17" s="20">
         <v>-3</v>
       </c>
-      <c r="H17" s="38">
+      <c r="H17" s="34">
         <v>6</v>
       </c>
-      <c r="I17" s="39">
+      <c r="I17" s="35">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="J17" s="39" t="str">
+      <c r="J17" s="35" t="str">
         <v>A2023</v>
       </c>
-      <c r="K17" s="39" t="str">
+      <c r="K17" s="35" t="str">
         <v>B2024</v>
       </c>
-      <c r="L17" s="40">
+      <c r="L17" s="36">
         <v>1</v>
       </c>
     </row>
@@ -2294,18 +2319,18 @@
       <c r="E18" s="32">
         <v>1</v>
       </c>
-      <c r="H18" s="38">
-        <v>7</v>
-      </c>
-      <c r="I18" s="39">
+      <c r="H18" s="34">
+        <v>7</v>
+      </c>
+      <c r="I18" s="35">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="J18" s="39" t="str">
+      <c r="J18" s="35" t="str">
         <v>C2023</v>
       </c>
-      <c r="K18" s="39"/>
-      <c r="L18" s="40"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="36"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A19" s="2"/>
@@ -2321,18 +2346,18 @@
       <c r="E19" s="21">
         <v>-1</v>
       </c>
-      <c r="H19" s="38">
+      <c r="H19" s="34">
         <v>8</v>
       </c>
-      <c r="I19" s="39">
+      <c r="I19" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J19" s="39" t="str">
+      <c r="J19" s="35" t="str">
         <v>B2024</v>
       </c>
-      <c r="K19" s="39"/>
-      <c r="L19" s="40"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="36"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A20" s="2"/>
@@ -2404,7 +2429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB0E197A-3FDB-417B-9D98-1DD72085D2B3}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
@@ -2422,18 +2447,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="H1" s="35" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="H1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -2596,7 +2621,7 @@
       <c r="E9" s="20">
         <v>7</v>
       </c>
-      <c r="H9" s="36" t="str" cm="1">
+      <c r="H9" s="33" t="str" cm="1">
         <f t="array" ref="H9:K12">_xlfn.LET(_xlpm.T,B3:E19,_xlpm.Y,YEAR(_xlfn.TAKE(_xlpm.T,,1)),_xlpm.O,_xlfn.CHOOSECOLS(_xlpm.T,2),_xlpm.P,_xlfn.CHOOSECOLS(_xlpm.T,3),_xlpm.Q,_xlfn.TAKE(_xlpm.T,,-1),_xlpm.UO,_xlfn.UNIQUE(_xlpm.O),_xlpm.QS,_xlfn.MAP(_xlpm.UO,_xlfn.LAMBDA(_xlpm.A,SUM(_xlfn._xlws.FILTER(_xlpm.Q,_xlpm.O=_xlpm.A)))),_xlpm.PY,_xlfn.MAP(_xlpm.UO,_xlfn.LAMBDA(_xlpm.A,_xlfn.TAKE((_xlfn._xlws.FILTER(_xlpm.P&amp;_xlpm.Y,_xlpm.O=_xlpm.A)),1))),_xlpm.UPY,_xlfn.UNIQUE(_xlpm.PY),_xlpm.UC,_xlfn.MAP(_xlpm.UPY,_xlfn.LAMBDA(_xlpm.A,SUM(_xlfn._xlws.FILTER(_xlpm.QS,_xlpm.PY=_xlpm.A)))),_xlpm.TUY,TRANSPOSE(_xlfn.UNIQUE(_xlpm.Y)),_xlpm.USP,_xlfn.UNIQUE(_xlfn._xlws.SORT(_xlpm.P)),_xlpm.X,_xlfn.XLOOKUP(_xlpm.USP&amp;_xlpm.TUY,_xlpm.UPY,_xlpm.UC,0),_xlfn.VSTACK(_xlfn.HSTACK("Product",_xlpm.TUY),_xlfn.HSTACK(_xlpm.USP,IF(_xlpm.X=0,"",_xlpm.X))))</f>
         <v>Product</v>
       </c>
@@ -2624,7 +2649,7 @@
       <c r="E10" s="27">
         <v>-2</v>
       </c>
-      <c r="H10" s="36" t="str">
+      <c r="H10" s="33" t="str">
         <v>A</v>
       </c>
       <c r="I10" s="3" t="str">
@@ -2651,7 +2676,7 @@
       <c r="E11" s="20">
         <v>-3</v>
       </c>
-      <c r="H11" s="37" t="str">
+      <c r="H11" s="3" t="str">
         <v>B</v>
       </c>
       <c r="I11" s="3" t="str">
@@ -2678,7 +2703,7 @@
       <c r="E12" s="20">
         <v>2</v>
       </c>
-      <c r="H12" s="37" t="str">
+      <c r="H12" s="3" t="str">
         <v>C</v>
       </c>
       <c r="I12" s="3">
@@ -2926,37 +2951,37 @@
       <c r="B27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
-      <c r="J27" s="43" t="s">
+      <c r="J27" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="K27" s="44" t="s">
+      <c r="K27" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="L27" s="44" t="s">
+      <c r="L27" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="M27" s="44" t="s">
+      <c r="M27" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="N27" s="45" t="s">
+      <c r="N27" s="41" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="21.6" thickTop="1" x14ac:dyDescent="0.4">
       <c r="I28" s="11"/>
-      <c r="J28" s="38">
-        <v>1</v>
-      </c>
-      <c r="K28" s="39">
+      <c r="J28" s="34">
+        <v>1</v>
+      </c>
+      <c r="K28" s="35">
         <v>0</v>
       </c>
-      <c r="L28" s="39" t="s">
+      <c r="L28" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="M28" s="39" t="s">
+      <c r="M28" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="N28" s="40">
+      <c r="N28" s="36">
         <v>0</v>
       </c>
     </row>
@@ -2965,37 +2990,37 @@
       <c r="B29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
-      <c r="J29" s="38">
+      <c r="J29" s="34">
         <v>2</v>
       </c>
-      <c r="K29" s="39">
-        <v>7</v>
-      </c>
-      <c r="L29" s="41" t="s">
+      <c r="K29" s="35">
+        <v>7</v>
+      </c>
+      <c r="L29" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="M29" s="39" t="s">
+      <c r="M29" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="N29" s="40">
+      <c r="N29" s="36">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A30" s="2"/>
-      <c r="J30" s="38">
+      <c r="J30" s="34">
         <v>3</v>
       </c>
-      <c r="K30" s="39">
+      <c r="K30" s="35">
         <v>0</v>
       </c>
-      <c r="L30" s="42" t="s">
+      <c r="L30" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="M30" s="39" t="s">
+      <c r="M30" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="N30" s="40">
+      <c r="N30" s="36">
         <v>0</v>
       </c>
     </row>
@@ -3003,82 +3028,82 @@
       <c r="A31" s="2"/>
       <c r="B31" s="6"/>
       <c r="D31" s="6"/>
-      <c r="J31" s="38">
+      <c r="J31" s="34">
         <v>4</v>
       </c>
-      <c r="K31" s="39">
+      <c r="K31" s="35">
         <v>0</v>
       </c>
-      <c r="L31" s="42" t="s">
+      <c r="L31" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="M31" s="39" t="s">
+      <c r="M31" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="N31" s="40">
+      <c r="N31" s="36">
         <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A32" s="2"/>
-      <c r="J32" s="38">
-        <v>5</v>
-      </c>
-      <c r="K32" s="39">
+      <c r="J32" s="34">
+        <v>5</v>
+      </c>
+      <c r="K32" s="35">
         <v>0</v>
       </c>
-      <c r="L32" s="41" t="s">
+      <c r="L32" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="M32" s="39" t="s">
+      <c r="M32" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="N32" s="40">
+      <c r="N32" s="36">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="10:14" x14ac:dyDescent="0.4">
-      <c r="J33" s="38">
+      <c r="J33" s="34">
         <v>6</v>
       </c>
-      <c r="K33" s="39">
+      <c r="K33" s="35">
         <v>4</v>
       </c>
-      <c r="L33" s="39" t="s">
+      <c r="L33" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="M33" s="39" t="s">
+      <c r="M33" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="N33" s="40">
+      <c r="N33" s="36">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="10:14" x14ac:dyDescent="0.4">
-      <c r="J34" s="38">
-        <v>7</v>
-      </c>
-      <c r="K34" s="39">
+      <c r="J34" s="34">
+        <v>7</v>
+      </c>
+      <c r="K34" s="35">
         <v>2</v>
       </c>
-      <c r="L34" s="39" t="s">
+      <c r="L34" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="M34" s="39"/>
-      <c r="N34" s="40"/>
+      <c r="M34" s="35"/>
+      <c r="N34" s="36"/>
     </row>
     <row r="35" spans="10:14" x14ac:dyDescent="0.4">
-      <c r="J35" s="38">
+      <c r="J35" s="34">
         <v>8</v>
       </c>
-      <c r="K35" s="39">
-        <v>1</v>
-      </c>
-      <c r="L35" s="39" t="s">
+      <c r="K35" s="35">
+        <v>1</v>
+      </c>
+      <c r="L35" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="M35" s="39"/>
-      <c r="N35" s="40"/>
+      <c r="M35" s="35"/>
+      <c r="N35" s="36"/>
     </row>
     <row r="36" spans="10:14" x14ac:dyDescent="0.4">
       <c r="N36" s="3" t="s">
@@ -3104,6 +3129,523 @@
       <c r="J40" s="3" t="s">
         <v>21</v>
       </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="H1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D8C1AB-46E3-4564-9595-3534456339E5}">
+  <dimension ref="A1:P32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="4.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19" style="3" customWidth="1"/>
+    <col min="3" max="4" width="12" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.8984375" style="3" customWidth="1"/>
+    <col min="6" max="7" width="20" style="3" customWidth="1"/>
+    <col min="8" max="8" width="11.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="8.19921875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="9" style="3"/>
+    <col min="13" max="13" width="16.09765625" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="H1" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A2" s="2"/>
+      <c r="B2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="16">
+        <v>2022</v>
+      </c>
+      <c r="J2" s="16">
+        <v>2023</v>
+      </c>
+      <c r="K2" s="17">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A3" s="2"/>
+      <c r="B3" s="22">
+        <v>44708</v>
+      </c>
+      <c r="C3" s="23">
+        <v>1</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="24">
+        <v>5</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4">
+        <v>4</v>
+      </c>
+      <c r="K3" s="18"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A4" s="2"/>
+      <c r="B4" s="12">
+        <v>44780</v>
+      </c>
+      <c r="C4" s="9">
+        <v>2</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="20">
+        <v>7</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="28"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A5" s="2"/>
+      <c r="B5" s="12">
+        <v>44812</v>
+      </c>
+      <c r="C5" s="9">
+        <v>3</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="20">
+        <v>2</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="7">
+        <v>7</v>
+      </c>
+      <c r="J5" s="7">
+        <v>2</v>
+      </c>
+      <c r="K5" s="19"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A6" s="2"/>
+      <c r="B6" s="12">
+        <v>44853</v>
+      </c>
+      <c r="C6" s="9">
+        <v>4</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A7" s="2"/>
+      <c r="B7" s="12">
+        <v>44917</v>
+      </c>
+      <c r="C7" s="9">
+        <v>5</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A8" s="2"/>
+      <c r="B8" s="12">
+        <v>44938</v>
+      </c>
+      <c r="C8" s="9">
+        <v>3</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="20">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A9" s="2"/>
+      <c r="B9" s="12">
+        <v>44991</v>
+      </c>
+      <c r="C9" s="9">
+        <v>6</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="20">
+        <v>7</v>
+      </c>
+      <c r="H9" s="14"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A10" s="2"/>
+      <c r="B10" s="25">
+        <v>45102</v>
+      </c>
+      <c r="C10" s="26">
+        <v>1</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="27">
+        <v>-2</v>
+      </c>
+      <c r="H10" s="14"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A11" s="2"/>
+      <c r="B11" s="12">
+        <v>45105</v>
+      </c>
+      <c r="C11" s="9">
+        <v>4</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="20">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A12" s="2"/>
+      <c r="B12" s="12">
+        <v>45139</v>
+      </c>
+      <c r="C12" s="9">
+        <v>7</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A13" s="2"/>
+      <c r="B13" s="25">
+        <v>45183</v>
+      </c>
+      <c r="C13" s="26">
+        <v>1</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="27">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A14" s="2"/>
+      <c r="B14" s="12">
+        <v>45489</v>
+      </c>
+      <c r="C14" s="9">
+        <v>3</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="20">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A15" s="2"/>
+      <c r="B15" s="12">
+        <v>45545</v>
+      </c>
+      <c r="C15" s="9">
+        <v>5</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="20">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A16" s="2"/>
+      <c r="B16" s="25">
+        <v>45569</v>
+      </c>
+      <c r="C16" s="26">
+        <v>1</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="27">
+        <v>-2</v>
+      </c>
+      <c r="H16" s="15" t="str" cm="1">
+        <f t="array" ref="H16:K19">_xlfn.LET(
+_xlpm.Y,   YEAR(_Y),_xlpm.O, _O,_xlpm.P, _P,_xlpm.Q, _Q,
+_xlpm.UO,  _xlfn.UNIQUE(_xlpm.O),
+_xlpm.QS,  _xlfn.MAP(_xlpm.UO, _xlfn.LAMBDA(_xlpm.x, SUM(_xlfn._xlws.FILTER(_xlpm.Q,_O=_xlpm.x)))),
+_xlpm.PY,  _xlfn.MAP(_xlpm.UO, _xlfn.LAMBDA(_xlpm.x, _xlfn.TAKE(_xlfn._xlws.FILTER(_xlpm.P&amp;_xlpm.Y,_O=_xlpm.x),1))),
+_xlpm.UPY, _xlfn.UNIQUE(_xlpm.PY),
+_xlpm.UC,  _xlfn.MAP(_xlpm.UPY, _xlfn.LAMBDA(_xlpm.x, SUM(_xlfn._xlws.FILTER(_xlpm.QS,_xlpm.PY=_xlpm.x)))),
+_xlpm.ZZ,  _xlfn.XLOOKUP(_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlpm.P))&amp;TRANSPOSE(_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlpm.Y))),_xlpm.UPY,_xlpm.UC,""),
+_xlfn.HSTACK(_xlfn.VSTACK("Product",_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlpm.P))),_xlfn.VSTACK(TRANSPOSE(_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlpm.Y))),_xlpm.ZZ))
+)</f>
+        <v>Product</v>
+      </c>
+      <c r="I16" s="16">
+        <v>2022</v>
+      </c>
+      <c r="J16" s="16">
+        <v>2023</v>
+      </c>
+      <c r="K16" s="17">
+        <v>2024</v>
+      </c>
+      <c r="M16" s="3" t="b" cm="1">
+        <f t="array" ref="M16:P19">_xlfn.ANCHORARRAY(H16)=H2:K5</f>
+        <v>1</v>
+      </c>
+      <c r="N16" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="O16" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="P16" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A17" s="2"/>
+      <c r="B17" s="12">
+        <v>45574</v>
+      </c>
+      <c r="C17" s="9">
+        <v>6</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="20">
+        <v>-3</v>
+      </c>
+      <c r="H17" s="4" t="str">
+        <v>A</v>
+      </c>
+      <c r="I17" s="46">
+        <v>0</v>
+      </c>
+      <c r="J17" s="46">
+        <v>4</v>
+      </c>
+      <c r="K17" s="47" t="str">
+        <v/>
+      </c>
+      <c r="M17" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="N17" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="O17" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="P17" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A18" s="2"/>
+      <c r="B18" s="30">
+        <v>45585</v>
+      </c>
+      <c r="C18" s="31">
+        <v>8</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="32">
+        <v>1</v>
+      </c>
+      <c r="H18" s="5" t="str">
+        <v>B</v>
+      </c>
+      <c r="I18" s="48">
+        <v>0</v>
+      </c>
+      <c r="J18" s="49" t="str">
+        <v/>
+      </c>
+      <c r="K18" s="50">
+        <v>1</v>
+      </c>
+      <c r="M18" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="N18" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="O18" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="P18" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A19" s="2"/>
+      <c r="B19" s="13">
+        <v>45648</v>
+      </c>
+      <c r="C19" s="10">
+        <v>5</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="21">
+        <v>-1</v>
+      </c>
+      <c r="H19" s="7" t="str">
+        <v>C</v>
+      </c>
+      <c r="I19" s="51">
+        <v>7</v>
+      </c>
+      <c r="J19" s="51">
+        <v>2</v>
+      </c>
+      <c r="K19" s="52" t="str">
+        <v/>
+      </c>
+      <c r="M19" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="N19" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="O19" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="P19" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A24" s="2"/>
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A25" s="2"/>
+      <c r="D25" s="6"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="I28" s="11"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A29" s="2"/>
+      <c r="B29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A31" s="2"/>
+      <c r="B31" s="6"/>
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A32" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
What I learned section
</commit_message>
<xml_diff>
--- a/CH-055 Warehouse Management_1.xlsx
+++ b/CH-055 Warehouse Management_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="14_{A6DC8524-85D4-4049-AFC2-E49ABD8B82CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F59CD413-7BF5-4D04-AA9F-72F0AD0CEC5E}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="14_{A6DC8524-85D4-4049-AFC2-E49ABD8B82CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE4A82AD-6AC4-4FF6-83DA-96667BB08748}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="30">
   <si>
     <t>Result</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>This is why the Take command is used to grab the first one.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The key observation here is that the first order is grabbed using take. </t>
+  </si>
+  <si>
+    <t>This makes everything else pretty straightword.</t>
   </si>
 </sst>
 </file>
@@ -678,6 +684,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -686,27 +713,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1419,18 +1425,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="H1" s="45" t="s">
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="H1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -1836,18 +1842,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="H1" s="45" t="s">
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="H1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -2107,15 +2113,15 @@
         <f t="array" ref="N12:N14">_xlfn._xlws.SORT(_xlfn.UNIQUE(LEFT(_xlfn.ANCHORARRAY(K12),1)))</f>
         <v>A</v>
       </c>
-      <c r="O12" s="46" cm="1">
+      <c r="O12" s="43" cm="1">
         <f t="array" ref="O12">_xlfn.XLOOKUP($N12&amp;O$11,_xlfn.ANCHORARRAY($K$12),_xlfn.ANCHORARRAY($L$12),"")</f>
         <v>0</v>
       </c>
-      <c r="P12" s="46" cm="1">
+      <c r="P12" s="43" cm="1">
         <f t="array" ref="P12">_xlfn.XLOOKUP($N12&amp;P$11,_xlfn.ANCHORARRAY($K$12),_xlfn.ANCHORARRAY($L$12),"")</f>
         <v>4</v>
       </c>
-      <c r="Q12" s="47" t="str" cm="1">
+      <c r="Q12" s="44" t="str" cm="1">
         <f t="array" ref="Q12">_xlfn.XLOOKUP($N12&amp;Q$11,_xlfn.ANCHORARRAY($K$12),_xlfn.ANCHORARRAY($L$12),"")</f>
         <v/>
       </c>
@@ -2153,15 +2159,15 @@
       <c r="N13" s="5" t="str">
         <v>B</v>
       </c>
-      <c r="O13" s="48" cm="1">
+      <c r="O13" s="45" cm="1">
         <f t="array" ref="O13">_xlfn.XLOOKUP($N13&amp;O$11,_xlfn.ANCHORARRAY($K$12),_xlfn.ANCHORARRAY($L$12),"")</f>
         <v>0</v>
       </c>
-      <c r="P13" s="49" t="str" cm="1">
+      <c r="P13" s="46" t="str" cm="1">
         <f t="array" ref="P13">_xlfn.XLOOKUP($N13&amp;P$11,_xlfn.ANCHORARRAY($K$12),_xlfn.ANCHORARRAY($L$12),"")</f>
         <v/>
       </c>
-      <c r="Q13" s="50" cm="1">
+      <c r="Q13" s="47" cm="1">
         <f t="array" ref="Q13">_xlfn.XLOOKUP($N13&amp;Q$11,_xlfn.ANCHORARRAY($K$12),_xlfn.ANCHORARRAY($L$12),"")</f>
         <v>1</v>
       </c>
@@ -2199,15 +2205,15 @@
       <c r="N14" s="7" t="str">
         <v>C</v>
       </c>
-      <c r="O14" s="51" cm="1">
+      <c r="O14" s="48" cm="1">
         <f t="array" ref="O14">_xlfn.XLOOKUP($N14&amp;O$11,_xlfn.ANCHORARRAY($K$12),_xlfn.ANCHORARRAY($L$12),"")</f>
         <v>7</v>
       </c>
-      <c r="P14" s="51" cm="1">
+      <c r="P14" s="48" cm="1">
         <f t="array" ref="P14">_xlfn.XLOOKUP($N14&amp;P$11,_xlfn.ANCHORARRAY($K$12),_xlfn.ANCHORARRAY($L$12),"")</f>
         <v>2</v>
       </c>
-      <c r="Q14" s="52" t="str" cm="1">
+      <c r="Q14" s="49" t="str" cm="1">
         <f t="array" ref="Q14">_xlfn.XLOOKUP($N14&amp;Q$11,_xlfn.ANCHORARRAY($K$12),_xlfn.ANCHORARRAY($L$12),"")</f>
         <v/>
       </c>
@@ -2447,18 +2453,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="H1" s="45" t="s">
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="H1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -3145,7 +3151,7 @@
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -3163,18 +3169,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="H1" s="45" t="s">
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="H1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -3384,6 +3390,9 @@
       <c r="E12" s="20">
         <v>2</v>
       </c>
+      <c r="H12" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A13" s="2"/>
@@ -3398,6 +3407,9 @@
       </c>
       <c r="E13" s="27">
         <v>-1</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.4">
@@ -3497,13 +3509,13 @@
       <c r="H17" s="4" t="str">
         <v>A</v>
       </c>
-      <c r="I17" s="46">
+      <c r="I17" s="43">
         <v>0</v>
       </c>
-      <c r="J17" s="46">
+      <c r="J17" s="43">
         <v>4</v>
       </c>
-      <c r="K17" s="47" t="str">
+      <c r="K17" s="44" t="str">
         <v/>
       </c>
       <c r="M17" s="3" t="b">
@@ -3536,13 +3548,13 @@
       <c r="H18" s="5" t="str">
         <v>B</v>
       </c>
-      <c r="I18" s="48">
+      <c r="I18" s="45">
         <v>0</v>
       </c>
-      <c r="J18" s="49" t="str">
+      <c r="J18" s="46" t="str">
         <v/>
       </c>
-      <c r="K18" s="50">
+      <c r="K18" s="47">
         <v>1</v>
       </c>
       <c r="M18" s="3" t="b">
@@ -3575,13 +3587,13 @@
       <c r="H19" s="7" t="str">
         <v>C</v>
       </c>
-      <c r="I19" s="51">
-        <v>7</v>
-      </c>
-      <c r="J19" s="51">
+      <c r="I19" s="48">
+        <v>7</v>
+      </c>
+      <c r="J19" s="48">
         <v>2</v>
       </c>
-      <c r="K19" s="52" t="str">
+      <c r="K19" s="49" t="str">
         <v/>
       </c>
       <c r="M19" s="3" t="b">

</xml_diff>